<commit_message>
cleaned up Sympy examples
</commit_message>
<xml_diff>
--- a/src/16 Scientific Libraries/07 Spreadsheets/data/writingToCells.xlsx
+++ b/src/16 Scientific Libraries/07 Spreadsheets/data/writingToCells.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="dd-mm-yyyy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -51,12 +50,80 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -359,7 +426,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n">
-        <v>43854.49782928298</v>
+        <v>44631.91980947088</v>
       </c>
       <c r="B1" t="n">
         <v>42</v>
@@ -564,572 +631,632 @@
       </c>
     </row>
     <row r="9">
-      <c r="B9" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" t="n">
-        <v>25</v>
-      </c>
-      <c r="H9" t="n">
-        <v>64</v>
-      </c>
-      <c r="K9" t="n">
-        <v>121</v>
-      </c>
-      <c r="N9" t="n">
-        <v>196</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>289</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2**2 = 4</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>5**2 = 25</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>8**2 = 64</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>11**2 = 121</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>14**2 = 196</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>17**2 = 289</t>
+        </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" t="n">
-        <v>25</v>
-      </c>
-      <c r="H10" t="n">
-        <v>64</v>
-      </c>
-      <c r="K10" t="n">
-        <v>121</v>
-      </c>
-      <c r="N10" t="n">
-        <v>196</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>289</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2**2 = 4</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>5**2 = 25</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>8**2 = 64</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>11**2 = 121</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>14**2 = 196</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>17**2 = 289</t>
+        </is>
       </c>
     </row>
     <row r="11">
-      <c r="B11" t="n">
-        <v>4</v>
-      </c>
-      <c r="E11" t="n">
-        <v>25</v>
-      </c>
-      <c r="H11" t="n">
-        <v>64</v>
-      </c>
-      <c r="K11" t="n">
-        <v>121</v>
-      </c>
-      <c r="N11" t="n">
-        <v>196</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>289</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2**2 = 4</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>5**2 = 25</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>8**2 = 64</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>11**2 = 121</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>14**2 = 196</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>17**2 = 289</t>
+        </is>
       </c>
     </row>
     <row r="12">
-      <c r="B12" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" t="n">
-        <v>25</v>
-      </c>
-      <c r="H12" t="n">
-        <v>64</v>
-      </c>
-      <c r="K12" t="n">
-        <v>121</v>
-      </c>
-      <c r="N12" t="n">
-        <v>196</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>289</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2**2 = 4</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>5**2 = 25</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>8**2 = 64</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>11**2 = 121</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>14**2 = 196</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>17**2 = 289</t>
+        </is>
       </c>
     </row>
     <row r="13">
-      <c r="B13" t="n">
-        <v>4</v>
-      </c>
-      <c r="E13" t="n">
-        <v>25</v>
-      </c>
-      <c r="H13" t="n">
-        <v>64</v>
-      </c>
-      <c r="K13" t="n">
-        <v>121</v>
-      </c>
-      <c r="N13" t="n">
-        <v>196</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>289</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2**2 = 4</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>5**2 = 25</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>8**2 = 64</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>11**2 = 121</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>14**2 = 196</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>17**2 = 289</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>--A--</t>
+          <t>cell A20</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>--B--</t>
+          <t>cell B20</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>--C--</t>
+          <t>cell C20</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>--D--</t>
+          <t>cell D20</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>--E--</t>
+          <t>cell E20</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>--F--</t>
+          <t>cell F20</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>--G--</t>
+          <t>cell G20</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>--H--</t>
+          <t>cell H20</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>--I--</t>
+          <t>cell I20</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>--A--</t>
+          <t>cell A21</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>--B--</t>
+          <t>cell B21</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>--C--</t>
+          <t>cell C21</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>--D--</t>
+          <t>cell D21</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>--E--</t>
+          <t>cell E21</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>--F--</t>
+          <t>cell F21</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>--G--</t>
+          <t>cell G21</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>--H--</t>
+          <t>cell H21</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>--I--</t>
+          <t>cell I21</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>--A--</t>
+          <t>cell A22</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>--B--</t>
+          <t>cell B22</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>--C--</t>
+          <t>cell C22</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>--D--</t>
+          <t>cell D22</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>--E--</t>
+          <t>cell E22</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>--F--</t>
+          <t>cell F22</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>--G--</t>
+          <t>cell G22</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>--H--</t>
+          <t>cell H22</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>--I--</t>
+          <t>cell I22</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>--A--</t>
+          <t>cell A23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>--B--</t>
+          <t>cell B23</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>--C--</t>
+          <t>cell C23</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>--D--</t>
+          <t>cell D23</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>--E--</t>
+          <t>cell E23</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>--F--</t>
+          <t>cell F23</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>--G--</t>
+          <t>cell G23</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>--H--</t>
+          <t>cell H23</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>--I--</t>
+          <t>cell I23</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>--A--</t>
+          <t>cell A24</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>--B--</t>
+          <t>cell B24</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>--C--</t>
+          <t>cell C24</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>--D--</t>
+          <t>cell D24</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>--E--</t>
+          <t>cell E24</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>--F--</t>
+          <t>cell F24</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>--G--</t>
+          <t>cell G24</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>--H--</t>
+          <t>cell H24</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>--I--</t>
+          <t>cell I24</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>--A--</t>
+          <t>cell A25</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>--B--</t>
+          <t>cell B25</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>--C--</t>
+          <t>cell C25</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>--D--</t>
+          <t>cell D25</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>--E--</t>
+          <t>cell E25</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>--F--</t>
+          <t>cell F25</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>--G--</t>
+          <t>cell G25</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>--H--</t>
+          <t>cell H25</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>--I--</t>
+          <t>cell I25</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>--A--</t>
+          <t>cell A26</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>--B--</t>
+          <t>cell B26</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>--C--</t>
+          <t>cell C26</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>--D--</t>
+          <t>cell D26</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>--E--</t>
+          <t>cell E26</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>--F--</t>
+          <t>cell F26</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>--G--</t>
+          <t>cell G26</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>--H--</t>
+          <t>cell H26</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>--I--</t>
+          <t>cell I26</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>--A--</t>
+          <t>cell A27</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>--B--</t>
+          <t>cell B27</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>--C--</t>
+          <t>cell C27</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>--D--</t>
+          <t>cell D27</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>--E--</t>
+          <t>cell E27</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>--F--</t>
+          <t>cell F27</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>--G--</t>
+          <t>cell G27</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>--H--</t>
+          <t>cell H27</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>--I--</t>
+          <t>cell I27</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>--A--</t>
+          <t>cell A28</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>--B--</t>
+          <t>cell B28</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>--C--</t>
+          <t>cell C28</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>--D--</t>
+          <t>cell D28</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>--E--</t>
+          <t>cell E28</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>--F--</t>
+          <t>cell F28</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>--G--</t>
+          <t>cell G28</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>--H--</t>
+          <t>cell H28</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>--I--</t>
+          <t>cell I28</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>--A--</t>
+          <t>cell A29</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>--B--</t>
+          <t>cell B29</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>--C--</t>
+          <t>cell C29</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>--D--</t>
+          <t>cell D29</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>--E--</t>
+          <t>cell E29</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>--F--</t>
+          <t>cell F29</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>--G--</t>
+          <t>cell G29</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>--H--</t>
+          <t>cell H29</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>--I--</t>
+          <t>cell I29</t>
         </is>
       </c>
     </row>

</xml_diff>